<commit_message>
Updated PPT anf spreadsheet
</commit_message>
<xml_diff>
--- a/src/HBB-did-url-spec-Low-level-Use Cases 0.3.xlsx
+++ b/src/HBB-did-url-spec-Low-level-Use Cases 0.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\INDY\did-url-spec\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74B95A1-D056-45DA-8260-1F1201108216}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A957D41-A704-4B43-A018-F7CCEB073D1C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{55C97778-1C7A-4748-8CBF-F07099F47EAB}"/>
   </bookViews>
@@ -24,8 +24,66 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Michael Herman</author>
+  </authors>
+  <commentList>
+    <comment ref="A53" authorId="0" shapeId="0" xr:uid="{3D7BF824-4FC8-4369-A65A-0F829B8AE973}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Herman:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A55" authorId="0" shapeId="0" xr:uid="{05B789F3-E10A-422E-87C5-4468951FB8CB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Michael Herman:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="127">
   <si>
     <t>did:xyz:1234</t>
   </si>
@@ -437,6 +495,18 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
+      <t/>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
       <t>Proposed `did-url` Syntax Example 1</t>
     </r>
     <r>
@@ -462,30 +532,27 @@
         <rFont val="Consolas"/>
         <family val="3"/>
       </rPr>
-      <t>Proposed `did-url` Syntax Example 2</t>
+      <t/>
     </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">
+  </si>
+  <si>
+    <t xml:space="preserve">Proposed `did-url` Syntax Example 2
 {
   "@type": "did:sov:BzCbsNYhMrjHiqZDTUASHg;spec/feature-discovery/1.0/request",
   "@id": "yWd8wfYzhmuXX3hmLNaV5bVbAjbWaU",
   "query": "did:sov:BzCbsNYhMrjHiqZDTUASHg!$filter='*'"
 }
 </t>
-    </r>
+  </si>
+  <si>
+    <t>J.  Indy feature-discovery 1.0 HIPE Use Cases (Old Example from HIPE)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -546,6 +613,19 @@
       <name val="Consolas"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -567,7 +647,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -611,11 +691,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -930,11 +1019,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA45131C-D45A-4CCB-AB34-792AD348A4B4}">
-  <dimension ref="A1:D53"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA45131C-D45A-4CCB-AB34-792AD348A4B4}">
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,12 +1056,12 @@
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
@@ -1059,12 +1148,12 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
@@ -1095,11 +1184,11 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
       <c r="D15" s="14"/>
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1117,11 +1206,11 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
       <c r="D18" s="14"/>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1223,11 +1312,11 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
       <c r="D27" s="14"/>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1272,12 +1361,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="15" t="s">
+    <row r="31" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="18" t="s">
         <v>112</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="13"/>
@@ -1285,11 +1374,11 @@
       <c r="D32" s="13"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
       <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1335,11 +1424,11 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="14"/>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1399,12 +1488,12 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="B44" s="14"/>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
+      <c r="B44" s="16"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="19"/>
     </row>
     <row r="45" spans="1:4" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
@@ -1435,11 +1524,11 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B48" s="14"/>
-      <c r="C48" s="14"/>
+      <c r="B48" s="16"/>
+      <c r="C48" s="16"/>
       <c r="D48" s="14"/>
     </row>
     <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1471,17 +1560,14 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="B52" s="14"/>
-      <c r="C52" s="14"/>
+      <c r="A52" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="B52" s="16"/>
+      <c r="C52" s="16"/>
       <c r="D52" s="14"/>
     </row>
-    <row r="53" spans="1:4" ht="293.25" x14ac:dyDescent="0.25">
-      <c r="A53" s="6">
-        <v>18</v>
-      </c>
+    <row r="53" spans="1:4" ht="102" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
         <v>114</v>
       </c>
@@ -1492,21 +1578,59 @@
         <v>115</v>
       </c>
     </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="16"/>
+      <c r="C54" s="16"/>
+      <c r="D54" s="14"/>
+    </row>
+    <row r="55" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="6">
+        <v>18</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="102" x14ac:dyDescent="0.25">
+      <c r="A56" s="6">
+        <v>19</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="A52:D52"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A44:D44"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="A33:D33"/>
+  <mergeCells count="12">
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A48:C48"/>
+    <mergeCell ref="A52:C52"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A27:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated presentation and spreadsheet
</commit_message>
<xml_diff>
--- a/src/HBB-did-url-spec-Low-level-Use Cases 0.3.xlsx
+++ b/src/HBB-did-url-spec-Low-level-Use Cases 0.3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\INDY\did-url-spec\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FAB33C7-EBB1-463C-ADE2-060CBD65BD84}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E8D9BC-56DB-4A89-9942-C7308690BB17}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{55C97778-1C7A-4748-8CBF-F07099F47EAB}"/>
   </bookViews>
@@ -383,9 +383,6 @@
     <t>did:xyz:1234!$exists</t>
   </si>
   <si>
-    <t>did:xyz:1234#key1!$exists</t>
-  </si>
-  <si>
     <t>http://uniresolver.io/did:xyz:1234!$exists</t>
   </si>
   <si>
@@ -552,6 +549,10 @@
   </si>
   <si>
     <t>Use case 11 moved to Category K</t>
+  </si>
+  <si>
+    <t>did:xyz:1234#key1!$exists
+did:xyz:1234!$exists="key1"</t>
   </si>
 </sst>
 </file>
@@ -703,20 +704,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1034,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA45131C-D45A-4CCB-AB34-792AD348A4B4}">
   <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1068,11 +1069,11 @@
       <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="16"/>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1160,11 +1161,11 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
       <c r="D11" s="15"/>
     </row>
     <row r="12" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1196,11 +1197,11 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
       <c r="D15" s="14"/>
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1218,11 +1219,11 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="A18" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="18"/>
       <c r="D18" s="14"/>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1236,7 +1237,7 @@
         <v>97</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1246,11 +1247,11 @@
       <c r="B20" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>98</v>
+      <c r="C20" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1261,10 +1262,10 @@
         <v>34</v>
       </c>
       <c r="C21" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1275,10 +1276,10 @@
         <v>35</v>
       </c>
       <c r="C22" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1289,10 +1290,10 @@
         <v>36</v>
       </c>
       <c r="C23" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1303,10 +1304,10 @@
         <v>37</v>
       </c>
       <c r="C24" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -1317,18 +1318,18 @@
         <v>38</v>
       </c>
       <c r="C25" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
       <c r="D27" s="14"/>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1364,23 +1365,23 @@
         <v>11</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D30" s="20" t="s">
+      <c r="D30" s="17" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
-      <c r="B31" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="C31" s="21"/>
+      <c r="B31" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="20"/>
       <c r="D31" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1389,11 +1390,11 @@
       <c r="D32" s="13"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
       <c r="D33" s="14"/>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1439,11 +1440,11 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+      <c r="A38" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="17"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="18"/>
       <c r="D38" s="14"/>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1503,11 +1504,11 @@
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
+      <c r="A44" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" s="18"/>
+      <c r="C44" s="18"/>
       <c r="D44" s="16"/>
     </row>
     <row r="45" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -1515,13 +1516,13 @@
         <v>54</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C45" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="C45" s="12" t="s">
-        <v>122</v>
-      </c>
       <c r="D45" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1529,21 +1530,21 @@
         <v>55</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="D46" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>120</v>
-      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="17"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
       <c r="D48" s="14"/>
     </row>
     <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1575,33 +1576,33 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="B52" s="17"/>
-      <c r="C52" s="17"/>
+      <c r="A52" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="B52" s="18"/>
+      <c r="C52" s="18"/>
       <c r="D52" s="14"/>
     </row>
     <row r="53" spans="1:4" ht="102" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="D53" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C54" s="12"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
+      <c r="A55" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" s="18"/>
+      <c r="C55" s="18"/>
       <c r="D55" s="14"/>
     </row>
     <row r="56" spans="1:4" ht="114.75" x14ac:dyDescent="0.25">
@@ -1609,13 +1610,13 @@
         <v>18</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D56" s="8" t="s">
         <v>114</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="D56" s="8" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="102" x14ac:dyDescent="0.25">
@@ -1623,21 +1624,21 @@
         <v>19</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C57" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="D57" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C57" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>115</v>
-      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="B58" s="17"/>
-      <c r="C58" s="17"/>
+      <c r="A58" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B58" s="18"/>
+      <c r="C58" s="18"/>
       <c r="D58" s="14"/>
     </row>
     <row r="59" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1645,7 +1646,7 @@
         <v>11</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C59" s="8" t="s">
         <v>76</v>
@@ -1655,10 +1656,10 @@
       </c>
     </row>
     <row r="60" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="C60" s="18"/>
+      <c r="B60" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" s="19"/>
       <c r="D60" s="1"/>
     </row>
   </sheetData>

</xml_diff>